<commit_message>
add editTutorial logic, test and handler in api; Add editTutorial logic in app and use it in Tutorial component in app #450
</commit_message>
<xml_diff>
--- a/staff/anna-cuenca/backend/api/Rito proceso.xlsx
+++ b/staff/anna-cuenca/backend/api/Rito proceso.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annacuencabocanegra/workspace/isdi-parttime-202309/staff/anna-cuenca/backend/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E7FEF6-C234-8144-8180-AB36EC77C4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB7133E-7C5D-0545-82C0-E419FBC9CF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43160" yWindow="2240" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
+    <workbookView xWindow="41280" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$E$138</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="149">
   <si>
     <t>Nombre</t>
   </si>
@@ -468,6 +471,21 @@
   </si>
   <si>
     <t>mov1,2,3, baile</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>FALTA</t>
+  </si>
+  <si>
+    <t>HECHO</t>
+  </si>
+  <si>
+    <t>MIERCOLES</t>
+  </si>
+  <si>
+    <t>FINDE</t>
   </si>
 </sst>
 </file>
@@ -517,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -525,11 +543,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -544,6 +571,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -866,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9F9D03-4CA4-564F-88AD-FCF0AD454CA7}">
-  <dimension ref="B2:E138"/>
+  <dimension ref="A2:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="137" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138:E138"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,59 +929,59 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>40</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>5</v>
+      <c r="D6" s="3">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>5</v>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -968,132 +999,132 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2">
-        <v>40</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>5</v>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2">
-        <v>20</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>5</v>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2">
-        <v>40</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>5</v>
+      <c r="D11" s="3">
+        <v>40</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2">
-        <v>20</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>5</v>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>50</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>5</v>
+      <c r="E13" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2">
-        <v>40</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>5</v>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2">
-        <v>20</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>5</v>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="2">
-        <v>40</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
+      <c r="D16" s="3">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="2">
-        <v>20</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1106,8 +1137,14 @@
       <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1121,7 +1158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1135,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1149,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1163,7 +1200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1177,7 +1214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1191,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1205,7 +1242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1219,7 +1256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1233,7 +1270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1247,7 +1284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1261,7 +1298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1275,7 +1312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1289,7 +1326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1303,7 +1340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1317,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1331,7 +1368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1345,7 +1382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1359,7 +1396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1373,7 +1410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1386,8 +1423,15 @@
       <c r="E38" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="6"/>
+      <c r="G38" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>44</v>
       </c>
@@ -1401,7 +1445,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>46</v>
       </c>
@@ -1415,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>47</v>
       </c>
@@ -1429,7 +1473,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>48</v>
       </c>
@@ -1443,7 +1487,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>49</v>
       </c>
@@ -1457,7 +1501,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>50</v>
       </c>
@@ -1471,7 +1515,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>51</v>
       </c>
@@ -1485,7 +1529,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
         <v>52</v>
       </c>
@@ -1499,7 +1543,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>53</v>
       </c>
@@ -1513,7 +1557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>54</v>
       </c>
@@ -2647,7 +2691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B129" s="3" t="s">
         <v>137</v>
       </c>
@@ -2661,7 +2705,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B130" s="3" t="s">
         <v>139</v>
       </c>
@@ -2675,7 +2719,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B131" s="3" t="s">
         <v>140</v>
       </c>
@@ -2689,7 +2733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B132" s="3" t="s">
         <v>141</v>
       </c>
@@ -2703,49 +2747,49 @@
         <v>45</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B133" s="2" t="s">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B133" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C133" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D133" s="5">
+      <c r="C133" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D133" s="7">
         <v>60</v>
       </c>
-      <c r="E133" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B134" s="2" t="s">
+      <c r="E133" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B134" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D134" s="5">
+      <c r="C134" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D134" s="7">
         <v>60</v>
       </c>
-      <c r="E134" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B135" s="2" t="s">
+      <c r="E134" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B135" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C135" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D135" s="5">
+      <c r="C135" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" s="7">
         <v>60</v>
       </c>
-      <c r="E135" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E135" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B136" s="2" t="s">
         <v>142</v>
       </c>
@@ -2758,8 +2802,15 @@
       <c r="E136" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F136" s="6"/>
+      <c r="G136" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
+      <c r="J136" s="6"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B137" s="2" t="s">
         <v>143</v>
       </c>
@@ -2773,7 +2824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B138" s="2" t="s">
         <v>142</v>
       </c>
@@ -2786,8 +2837,51 @@
       <c r="E138" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+      <c r="J138" s="6"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>144</v>
+      </c>
+      <c r="D141">
+        <f>SUM(D4:D138)</f>
+        <v>7290</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>146</v>
+      </c>
+      <c r="D143">
+        <f>SUM(D39:D47,D49:D52,D54:D57,D59:D62,D65:D70,D72:D80,D82:D85,D87:D90,D92:D100,D102:D105,D107:D132,D133:D135,D4:D7,D9:D17,)</f>
+        <v>5210</v>
+      </c>
+      <c r="E143">
+        <f>(D143/D141)*100</f>
+        <v>71.467764060356657</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>145</v>
+      </c>
+      <c r="D144">
+        <f>SUM(D135:D138,D106,D101,D91,D86,D81,D71,D63,D58,D53,D48,D18:D38,D8)</f>
+        <v>2140</v>
+      </c>
+      <c r="E144">
+        <f>(D144/D141)*100</f>
+        <v>29.355281207133061</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:E138" xr:uid="{1B9F9D03-4CA4-564F-88AD-FCF0AD454CA7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add snakeMove to the sequence of movements, in both app and API #456
</commit_message>
<xml_diff>
--- a/staff/anna-cuenca/backend/api/Rito proceso.xlsx
+++ b/staff/anna-cuenca/backend/api/Rito proceso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annacuencabocanegra/workspace/isdi-parttime-202309/staff/anna-cuenca/backend/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB7133E-7C5D-0545-82C0-E419FBC9CF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F3F505-BE2A-6F4C-9869-6D5435134409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41280" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
+    <workbookView xWindow="40160" yWindow="940" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$E$138</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="149">
   <si>
     <t>Nombre</t>
   </si>
@@ -601,9 +601,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -641,7 +641,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -747,7 +747,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -889,7 +889,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9F9D03-4CA4-564F-88AD-FCF0AD454CA7}">
   <dimension ref="A2:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2789,7 +2789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B136" s="2" t="s">
         <v>142</v>
       </c>
@@ -2802,13 +2802,6 @@
       <c r="E136" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F136" s="6"/>
-      <c r="G136" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H136" s="6"/>
-      <c r="I136" s="6"/>
-      <c r="J136" s="6"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B137" s="2" t="s">

</xml_diff>

<commit_message>
implement changeEmail spec in api #467
</commit_message>
<xml_diff>
--- a/staff/anna-cuenca/backend/api/Rito proceso.xlsx
+++ b/staff/anna-cuenca/backend/api/Rito proceso.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annacuencabocanegra/workspace/isdi-parttime-202309/staff/anna-cuenca/backend/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F3F505-BE2A-6F4C-9869-6D5435134409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE5B97C-4EB7-3541-8B30-9E0447B5EA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40160" yWindow="940" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
+    <workbookView xWindow="2580" yWindow="860" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$E$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$E$140</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="152">
   <si>
     <t>Nombre</t>
   </si>
@@ -482,10 +482,19 @@
     <t>HECHO</t>
   </si>
   <si>
-    <t>MIERCOLES</t>
-  </si>
-  <si>
-    <t>FINDE</t>
+    <t>Tailwind</t>
+  </si>
+  <si>
+    <t>Dar estilo a la app</t>
+  </si>
+  <si>
+    <t>Refactor</t>
+  </si>
+  <si>
+    <t>Optimitzar código</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -535,7 +544,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -543,20 +552,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,7 +573,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -897,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9F9D03-4CA4-564F-88AD-FCF0AD454CA7}">
-  <dimension ref="A2:J144"/>
+  <dimension ref="A2:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="L136" sqref="L136"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="140" workbookViewId="0">
+      <selection activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,7 +1064,7 @@
         <v>50</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -1110,7 +1109,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1137,70 +1136,64 @@
       <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
         <v>60</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="2">
-        <v>20</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3">
+        <v>20</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="2">
-        <v>40</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="D21" s="3">
+        <v>40</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="2">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3">
+        <v>20</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1214,63 +1207,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3">
         <v>60</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+      <c r="E24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="2">
-        <v>20</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3">
+        <v>20</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="2">
-        <v>40</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+      <c r="D26" s="3">
+        <v>40</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="2">
-        <v>20</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3">
+        <v>20</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1284,63 +1277,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="3">
         <v>60</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
+      <c r="E29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="2">
-        <v>20</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="s">
+      <c r="C30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3">
+        <v>20</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="2">
-        <v>40</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="2" t="s">
+      <c r="D31" s="3">
+        <v>40</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="2">
-        <v>20</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3">
+        <v>20</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1354,7 +1347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1368,7 +1361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1382,7 +1375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1396,7 +1389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1410,7 +1403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1423,15 +1416,8 @@
       <c r="E38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>44</v>
       </c>
@@ -1445,7 +1431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>46</v>
       </c>
@@ -1459,7 +1445,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>47</v>
       </c>
@@ -1473,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>48</v>
       </c>
@@ -1487,7 +1473,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>49</v>
       </c>
@@ -1501,7 +1487,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>50</v>
       </c>
@@ -1515,7 +1501,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>51</v>
       </c>
@@ -1529,7 +1515,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
         <v>52</v>
       </c>
@@ -1543,7 +1529,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>53</v>
       </c>
@@ -1557,7 +1543,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>54</v>
       </c>
@@ -2691,7 +2677,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B129" s="3" t="s">
         <v>137</v>
       </c>
@@ -2705,7 +2691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B130" s="3" t="s">
         <v>139</v>
       </c>
@@ -2719,7 +2705,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B131" s="3" t="s">
         <v>140</v>
       </c>
@@ -2733,7 +2719,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B132" s="3" t="s">
         <v>141</v>
       </c>
@@ -2747,63 +2733,63 @@
         <v>45</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B133" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C133" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D133" s="7">
+      <c r="C133" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D133" s="6">
         <v>60</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B134" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D134" s="7">
+      <c r="C134" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D134" s="6">
         <v>60</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B135" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C135" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D135" s="7">
+      <c r="C135" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" s="6">
         <v>60</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B136" s="2" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C136" s="5" t="s">
+      <c r="C136" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D136" s="5">
+      <c r="D136" s="6">
         <v>240</v>
       </c>
-      <c r="E136" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E136" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B137" s="2" t="s">
         <v>143</v>
       </c>
@@ -2817,64 +2803,85 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B138" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D138" s="5">
+        <v>1200</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B139" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D139" s="6">
+        <v>300</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C140" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D138" s="5">
+      <c r="D140" s="6">
         <v>240</v>
       </c>
-      <c r="E138" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="6"/>
-      <c r="G138" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H138" s="6"/>
-      <c r="I138" s="6"/>
-      <c r="J138" s="6"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="E140" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>144</v>
       </c>
-      <c r="D141">
-        <f>SUM(D4:D138)</f>
-        <v>7290</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="D143">
+        <f>SUM(D4:D140)</f>
+        <v>8790</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>146</v>
       </c>
-      <c r="D143">
-        <f>SUM(D39:D47,D49:D52,D54:D57,D59:D62,D65:D70,D72:D80,D82:D85,D87:D90,D92:D100,D102:D105,D107:D132,D133:D135,D4:D7,D9:D17,)</f>
-        <v>5210</v>
-      </c>
-      <c r="E143">
-        <f>(D143/D141)*100</f>
-        <v>71.467764060356657</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+      <c r="D145">
+        <f>SUM(D39:D47,D49:D52,D54:D57,D59:D62,D65:D70,D72:D80,D82:D85,D87:D90,D92:D100,D102:D105,D107:D132,D133:D136,D4:D7,D9:D12,D29:D32,D24:D27,D19:D22,D14:D17,D139:D140,D13)</f>
+        <v>6410</v>
+      </c>
+      <c r="E145">
+        <f>(D145/D143)*100</f>
+        <v>72.923777019340164</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>145</v>
       </c>
-      <c r="D144">
-        <f>SUM(D135:D138,D106,D101,D91,D86,D81,D71,D63,D58,D53,D48,D18:D38,D8)</f>
-        <v>2140</v>
-      </c>
-      <c r="E144">
-        <f>(D144/D141)*100</f>
-        <v>29.355281207133061</v>
+      <c r="D146">
+        <f>SUM(D137:D138,D106,D101,D91,D86,D81,D71,D63,D58,D53,D48,D33:D38,D8,D18,D23,D28)</f>
+        <v>2380</v>
+      </c>
+      <c r="E146">
+        <f>(D146/D143)*100</f>
+        <v>27.076222980659843</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:E138" xr:uid="{1B9F9D03-4CA4-564F-88AD-FCF0AD454CA7}"/>
+  <autoFilter ref="B2:E140" xr:uid="{1B9F9D03-4CA4-564F-88AD-FCF0AD454CA7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
clean and refactor #215; add custom buttons #436
</commit_message>
<xml_diff>
--- a/staff/anna-cuenca/backend/api/Rito proceso.xlsx
+++ b/staff/anna-cuenca/backend/api/Rito proceso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annacuencabocanegra/workspace/isdi-parttime-202309/staff/anna-cuenca/backend/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE5B97C-4EB7-3541-8B30-9E0447B5EA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AC44CD-3AA8-0640-AE1C-2F811569A872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="860" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
+    <workbookView xWindow="37880" yWindow="540" windowWidth="28040" windowHeight="17440" xr2:uid="{D1F81E76-B3AE-B24A-8F6B-690E76CF1F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="153">
   <si>
     <t>Nombre</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>hecho</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,12 +540,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEF913D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -556,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -565,9 +562,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -898,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9F9D03-4CA4-564F-88AD-FCF0AD454CA7}">
   <dimension ref="A2:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H143" sqref="H143"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,17 +978,17 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>50</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>5</v>
+      <c r="E8" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -1124,17 +1118,17 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>50</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>5</v>
+      <c r="E18" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -1194,16 +1188,16 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="3">
         <v>50</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1264,16 +1258,16 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="3">
         <v>50</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1334,86 +1328,86 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="3">
         <v>50</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="3">
         <v>60</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="2">
-        <v>20</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="B35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3">
+        <v>20</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="2">
-        <v>40</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="D36" s="3">
+        <v>40</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="2">
-        <v>20</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="C37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="3">
+        <v>20</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="3">
         <v>50</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1544,16 +1538,16 @@
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="3">
         <v>50</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1614,16 +1608,16 @@
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="3">
         <v>50</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1684,16 +1678,16 @@
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="3">
         <v>50</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1754,30 +1748,30 @@
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="3">
         <v>50</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D64" s="3">
         <v>0</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1866,16 +1860,16 @@
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="3">
         <v>50</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2006,16 +2000,16 @@
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="3">
         <v>50</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2076,16 +2070,16 @@
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="3">
         <v>50</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E86" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2146,16 +2140,16 @@
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="3">
         <v>50</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E91" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2286,16 +2280,16 @@
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101" s="3">
         <v>50</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2356,16 +2350,16 @@
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D106" s="3">
         <v>50</v>
       </c>
-      <c r="E106" s="2" t="s">
+      <c r="E106" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2737,10 +2731,10 @@
       <c r="B133" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C133" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D133" s="6">
+      <c r="C133" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D133" s="5">
         <v>60</v>
       </c>
       <c r="E133" s="3" t="s">
@@ -2751,10 +2745,10 @@
       <c r="B134" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D134" s="6">
+      <c r="C134" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D134" s="5">
         <v>60</v>
       </c>
       <c r="E134" s="3" t="s">
@@ -2765,10 +2759,10 @@
       <c r="B135" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C135" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D135" s="6">
+      <c r="C135" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" s="5">
         <v>60</v>
       </c>
       <c r="E135" s="3" t="s">
@@ -2779,10 +2773,10 @@
       <c r="B136" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C136" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D136" s="6">
+      <c r="D136" s="5">
         <v>240</v>
       </c>
       <c r="E136" s="3" t="s">
@@ -2790,7 +2784,7 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="3" t="s">
         <v>143</v>
       </c>
       <c r="C137" s="5" t="s">
@@ -2807,13 +2801,13 @@
       <c r="B138" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C138" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D138" s="5">
-        <v>1200</v>
-      </c>
-      <c r="E138" s="5" t="s">
+      <c r="D138" s="4">
+        <v>200</v>
+      </c>
+      <c r="E138" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2821,13 +2815,13 @@
       <c r="B139" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C139" s="6" t="s">
+      <c r="C139" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D139" s="6">
+      <c r="D139" s="5">
         <v>300</v>
       </c>
-      <c r="E139" s="6" t="s">
+      <c r="E139" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2835,13 +2829,13 @@
       <c r="B140" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C140" s="6" t="s">
+      <c r="C140" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D140" s="6">
+      <c r="D140" s="5">
         <v>240</v>
       </c>
-      <c r="E140" s="6" t="s">
+      <c r="E140" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2851,7 +2845,7 @@
       </c>
       <c r="D143">
         <f>SUM(D4:D140)</f>
-        <v>8790</v>
+        <v>7790</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -2859,12 +2853,12 @@
         <v>146</v>
       </c>
       <c r="D145">
-        <f>SUM(D39:D47,D49:D52,D54:D57,D59:D62,D65:D70,D72:D80,D82:D85,D87:D90,D92:D100,D102:D105,D107:D132,D133:D136,D4:D7,D9:D12,D29:D32,D24:D27,D19:D22,D14:D17,D139:D140,D13)</f>
-        <v>6410</v>
+        <f>SUM(D4:D137,D139:D140)</f>
+        <v>7590</v>
       </c>
       <c r="E145">
         <f>(D145/D143)*100</f>
-        <v>72.923777019340164</v>
+        <v>97.432605905006426</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -2873,11 +2867,11 @@
       </c>
       <c r="D146">
         <f>SUM(D137:D138,D106,D101,D91,D86,D81,D71,D63,D58,D53,D48,D33:D38,D8,D18,D23,D28)</f>
-        <v>2380</v>
+        <v>1380</v>
       </c>
       <c r="E146">
         <f>(D146/D143)*100</f>
-        <v>27.076222980659843</v>
+        <v>17.715019255455715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>